<commit_message>
Dodane wykresy w excelu.
</commit_message>
<xml_diff>
--- a/01/solution/dfs.xlsx
+++ b/01/solution/dfs.xlsx
@@ -32,7 +32,6 @@
     <definedName name="dfs_level10" localSheetId="1">'10'!$A$119:$K$233</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1987,23 +1986,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="dfs_level07" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\Lukasz\SkyDrive\Eclipse Workspace\15 - Spring 2014\SISE 01\solution\dfs_level07.txt" thousands="'"/>
-  </connection>
-  <connection id="4" name="dfs_level08" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\Lukasz\SkyDrive\Eclipse Workspace\15 - Spring 2014\SISE 01\solution\dfs_level08.txt" thousands="'"/>
-  </connection>
-  <connection id="5" name="dfs_level09" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\Lukasz\SkyDrive\Eclipse Workspace\15 - Spring 2014\SISE 01\solution\dfs_level09.txt" thousands="'"/>
-  </connection>
-  <connection id="6" name="dfs_level10" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\Lukasz\SkyDrive\Eclipse Workspace\15 - Spring 2014\SISE 01\solution\dfs_level10.txt" thousands="'"/>
-  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4093" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4099" uniqueCount="859">
   <si>
     <t>czas</t>
   </si>
@@ -4565,6 +4552,21 @@
   </si>
   <si>
     <t>[1, 2, 7, 3, 5, 6, 11, 4, 0, 10, 15, 8, 9, 13, 14, 12]</t>
+  </si>
+  <si>
+    <t>użyta pamięć2</t>
+  </si>
+  <si>
+    <t>użyta pamięć4</t>
+  </si>
+  <si>
+    <t>użyta pamięć5</t>
+  </si>
+  <si>
+    <t>użyta pamięć6</t>
+  </si>
+  <si>
+    <t>użyta pamięć7</t>
   </si>
 </sst>
 </file>
@@ -5100,21 +5102,30 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="118">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -5433,10 +5444,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5574,11 +5594,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520032192"/>
-        <c:axId val="529383424"/>
+        <c:axId val="48010304"/>
+        <c:axId val="517109376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520032192"/>
+        <c:axId val="48010304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5588,12 +5608,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="529383424"/>
+        <c:crossAx val="517109376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529383424"/>
+        <c:axId val="517109376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5604,7 +5624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520032192"/>
+        <c:crossAx val="48010304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5752,11 +5772,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="529385152"/>
-        <c:axId val="529385728"/>
+        <c:axId val="517120000"/>
+        <c:axId val="517120576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="529385152"/>
+        <c:axId val="517120000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5766,12 +5786,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="529385728"/>
+        <c:crossAx val="517120576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="529385728"/>
+        <c:axId val="517120576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5782,7 +5802,185 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="529385152"/>
+        <c:crossAx val="517120000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Podsumowanie!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>czas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podsumowanie!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podsumowanie!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.9999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4153999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8198333333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1274999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5031869158878504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3910762711864413</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6636806722689075</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6116160714285712</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8902521739130433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="533916480"/>
+        <c:axId val="533915904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="533916480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="533915904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533915904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="533916480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5866,231 +6064,251 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level10" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level02" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level09_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level08" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level07" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level02" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dfs_level01" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:D13" totalsRowShown="0">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:J13" totalsRowShown="0">
+  <tableColumns count="9">
     <tableColumn id="4" name="poziom trudności"/>
-    <tableColumn id="1" name="liczba operacji" dataDxfId="111">
+    <tableColumn id="1" name="liczba operacji" dataDxfId="7">
       <calculatedColumnFormula>AVERAGE(Table01[liczba operacji])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="użyta pamięć" dataDxfId="110"/>
+    <tableColumn id="2" name="użyta pamięć" dataDxfId="6"/>
+    <tableColumn id="3" name="użyta pamięć2" dataDxfId="5"/>
+    <tableColumn id="5" name="czas" dataDxfId="4"/>
+    <tableColumn id="6" name="użyta pamięć4" dataDxfId="3"/>
+    <tableColumn id="7" name="użyta pamięć5" dataDxfId="2"/>
+    <tableColumn id="8" name="użyta pamięć6" dataDxfId="1"/>
+    <tableColumn id="9" name="użyta pamięć7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table02" displayName="Table02" ref="A1:J5" totalsRowShown="0" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table02" displayName="Table02" ref="A1:J5" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="A1:J5"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="25"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="24"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="23"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="22"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="21"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="20"/>
-    <tableColumn id="7" name="czas" dataDxfId="19"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="18"/>
-    <tableColumn id="9" name="error" dataDxfId="17"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="16"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="28"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="27"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="26"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="25"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="24"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="23"/>
+    <tableColumn id="7" name="czas" dataDxfId="22"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="21"/>
+    <tableColumn id="9" name="error" dataDxfId="20"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table01" displayName="Table01" ref="A1:J3" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table01" displayName="Table01" ref="A1:J3" totalsRowShown="0" dataDxfId="18">
   <autoFilter ref="A1:J3"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="14"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="13"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="12"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="11"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="10"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="9"/>
-    <tableColumn id="7" name="czas" dataDxfId="8"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="7"/>
-    <tableColumn id="9" name="error" dataDxfId="6"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="5"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="17"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="16"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="15"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="14"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="13"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="12"/>
+    <tableColumn id="7" name="czas" dataDxfId="11"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="10"/>
+    <tableColumn id="9" name="error" dataDxfId="9"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table10" displayName="Table10" ref="A1:J116" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table10" displayName="Table10" ref="A1:J116" totalsRowShown="0" dataDxfId="117">
   <autoFilter ref="A1:J116"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="109"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="108"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="107"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="106"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="105"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="104"/>
-    <tableColumn id="7" name="czas" dataDxfId="103"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="102"/>
-    <tableColumn id="9" name="error" dataDxfId="101"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="100"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="116"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="115"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="114"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="113"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="112"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="111"/>
+    <tableColumn id="7" name="czas" dataDxfId="110"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="109"/>
+    <tableColumn id="9" name="error" dataDxfId="108"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table09" displayName="Table09" ref="A1:J116" totalsRowShown="0" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table09" displayName="Table09" ref="A1:J116" totalsRowShown="0" dataDxfId="106">
   <autoFilter ref="A1:J116"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="98"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="97"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="96"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="95"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="94"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="93"/>
-    <tableColumn id="7" name="czas" dataDxfId="92"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="91"/>
-    <tableColumn id="9" name="error" dataDxfId="90"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="89"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="105"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="104"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="103"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="102"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="101"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="100"/>
+    <tableColumn id="7" name="czas" dataDxfId="99"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="98"/>
+    <tableColumn id="9" name="error" dataDxfId="97"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table08" displayName="Table08" ref="A1:J120" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table08" displayName="Table08" ref="A1:J120" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="A1:J120"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="88"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="87"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="86"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="85"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="84"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="83"/>
-    <tableColumn id="7" name="czas" dataDxfId="82"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="81"/>
-    <tableColumn id="9" name="error" dataDxfId="80"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="79"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="94"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="93"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="92"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="91"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="90"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="89"/>
+    <tableColumn id="7" name="czas" dataDxfId="88"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="87"/>
+    <tableColumn id="9" name="error" dataDxfId="86"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table07" displayName="Table07" ref="A1:J119" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table07" displayName="Table07" ref="A1:J119" totalsRowShown="0" dataDxfId="84">
   <autoFilter ref="A1:J119"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="78"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="77"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="76"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="75"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="74"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="73"/>
-    <tableColumn id="7" name="czas" dataDxfId="72"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="71"/>
-    <tableColumn id="9" name="error" dataDxfId="70"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="69"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="83"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="82"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="81"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="80"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="79"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="78"/>
+    <tableColumn id="7" name="czas" dataDxfId="77"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="76"/>
+    <tableColumn id="9" name="error" dataDxfId="75"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table06" displayName="Table06" ref="A1:J108" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table06" displayName="Table06" ref="A1:J108" totalsRowShown="0" dataDxfId="73">
   <autoFilter ref="A1:J108"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="68"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="67"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="66"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="65"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="64"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="63"/>
-    <tableColumn id="7" name="czas" dataDxfId="62"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="61"/>
-    <tableColumn id="9" name="error" dataDxfId="60"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="59"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="72"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="71"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="70"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="69"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="68"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="67"/>
+    <tableColumn id="7" name="czas" dataDxfId="66"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="65"/>
+    <tableColumn id="9" name="error" dataDxfId="64"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table05" displayName="Table05" ref="A1:J55" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table05" displayName="Table05" ref="A1:J55" totalsRowShown="0" dataDxfId="62">
   <autoFilter ref="A1:J55"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="58"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="57"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="56"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="55"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="54"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="53"/>
-    <tableColumn id="7" name="czas" dataDxfId="52"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="51"/>
-    <tableColumn id="9" name="error" dataDxfId="50"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="49"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="61"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="60"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="59"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="58"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="57"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="56"/>
+    <tableColumn id="7" name="czas" dataDxfId="55"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="54"/>
+    <tableColumn id="9" name="error" dataDxfId="53"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table04" displayName="Table04" ref="A1:J25" totalsRowShown="0" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table04" displayName="Table04" ref="A1:J25" totalsRowShown="0" dataDxfId="51">
   <autoFilter ref="A1:J25"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="47"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="46"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="45"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="44"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="43"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="42"/>
-    <tableColumn id="7" name="czas" dataDxfId="41"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="40"/>
-    <tableColumn id="9" name="error" dataDxfId="39"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="38"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="50"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="49"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="48"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="47"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="46"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="45"/>
+    <tableColumn id="7" name="czas" dataDxfId="44"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="43"/>
+    <tableColumn id="9" name="error" dataDxfId="42"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table03" displayName="Table03" ref="A1:J11" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table03" displayName="Table03" ref="A1:J11" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="A1:J11"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="stan początkowy" dataDxfId="36"/>
-    <tableColumn id="2" name="algorytm" dataDxfId="35"/>
-    <tableColumn id="3" name="heurystyka" dataDxfId="34"/>
-    <tableColumn id="4" name="liczba operacji" dataDxfId="33"/>
-    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="32"/>
-    <tableColumn id="6" name="zajęta pamięć" dataDxfId="31"/>
-    <tableColumn id="7" name="czas" dataDxfId="30"/>
-    <tableColumn id="8" name="liczba króków" dataDxfId="29"/>
-    <tableColumn id="9" name="error" dataDxfId="28"/>
-    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="27"/>
+    <tableColumn id="1" name="stan początkowy" dataDxfId="39"/>
+    <tableColumn id="2" name="algorytm" dataDxfId="38"/>
+    <tableColumn id="3" name="heurystyka" dataDxfId="37"/>
+    <tableColumn id="4" name="liczba operacji" dataDxfId="36"/>
+    <tableColumn id="5" name="liczba przebytych węzłów" dataDxfId="35"/>
+    <tableColumn id="6" name="zajęta pamięć" dataDxfId="34"/>
+    <tableColumn id="7" name="czas" dataDxfId="33"/>
+    <tableColumn id="8" name="liczba króków" dataDxfId="32"/>
+    <tableColumn id="9" name="error" dataDxfId="31"/>
+    <tableColumn id="10" name="znaleziona ścieżka" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6383,10 +6601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D13"/>
+  <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F3" activeCellId="1" sqref="B3:B13 F3:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6394,7 +6612,7 @@
     <col min="2" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -6404,8 +6622,26 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>854</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>855</v>
+      </c>
+      <c r="H3" t="s">
+        <v>856</v>
+      </c>
+      <c r="I3" t="s">
+        <v>857</v>
+      </c>
+      <c r="J3" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -6417,8 +6653,32 @@
         <f>AVERAGE(Table01[liczba przebytych węzłów])</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="e">
+        <f>AVERAGE(Table01[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="2">
+        <f>AVERAGE(Table01[czas])</f>
+        <v>4.9999999999999992E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <f>AVERAGE(Table01[liczba króków])</f>
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="e">
+        <f>AVERAGE(Table01[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="2" t="e">
+        <f>AVERAGE(Table01[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <f>AVERAGE(Table01[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -6430,8 +6690,32 @@
         <f>AVERAGE(Table02[liczba przebytych węzłów])</f>
         <v>61951.75</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="e">
+        <f>AVERAGE(Table02[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="2">
+        <f>AVERAGE(Table02[czas])</f>
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <f>AVERAGE(Table02[liczba króków])</f>
+        <v>468.5</v>
+      </c>
+      <c r="H5" s="2" t="e">
+        <f>AVERAGE(Table02[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="2" t="e">
+        <f>AVERAGE(Table02[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <f>AVERAGE(Table02[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -6443,8 +6727,32 @@
         <f>AVERAGE(Table03[liczba przebytych węzłów])</f>
         <v>124339</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="e">
+        <f>AVERAGE(Table03[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="2">
+        <f>AVERAGE(Table03[czas])</f>
+        <v>1.4153999999999998</v>
+      </c>
+      <c r="G6" s="2">
+        <f>AVERAGE(Table03[liczba króków])</f>
+        <v>14494.2</v>
+      </c>
+      <c r="H6" s="2" t="e">
+        <f>AVERAGE(Table03[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="2" t="e">
+        <f>AVERAGE(Table03[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <f>AVERAGE(Table03[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -6456,8 +6764,32 @@
         <f>AVERAGE(Table04[liczba przebytych węzłów])</f>
         <v>181037.95833333334</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="e">
+        <f>AVERAGE(Table04[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="2">
+        <f>AVERAGE(Table04[czas])</f>
+        <v>1.8198333333333332</v>
+      </c>
+      <c r="G7" s="2">
+        <f>AVERAGE(Table04[liczba króków])</f>
+        <v>5388.5</v>
+      </c>
+      <c r="H7" s="2" t="e">
+        <f>AVERAGE(Table04[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="2" t="e">
+        <f>AVERAGE(Table04[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <f>AVERAGE(Table04[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -6469,8 +6801,32 @@
         <f>AVERAGE(Table05[liczba przebytych węzłów])</f>
         <v>195536.37037037036</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="e">
+        <f>AVERAGE(Table05[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="2">
+        <f>AVERAGE(Table05[czas])</f>
+        <v>2.1274999999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <f>AVERAGE(Table05[liczba króków])</f>
+        <v>5610.3148148148148</v>
+      </c>
+      <c r="H8" s="2" t="e">
+        <f>AVERAGE(Table05[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="2" t="e">
+        <f>AVERAGE(Table05[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <f>AVERAGE(Table05[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -6482,8 +6838,32 @@
         <f>AVERAGE(Table06[liczba przebytych węzłów])</f>
         <v>233053.07476635513</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="e">
+        <f>AVERAGE(Table06[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="2">
+        <f>AVERAGE(Table06[czas])</f>
+        <v>2.5031869158878504</v>
+      </c>
+      <c r="G9" s="2">
+        <f>AVERAGE(Table06[liczba króków])</f>
+        <v>5640.0373831775705</v>
+      </c>
+      <c r="H9" s="2" t="e">
+        <f>AVERAGE(Table06[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="2" t="e">
+        <f>AVERAGE(Table06[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <f>AVERAGE(Table06[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -6495,8 +6875,32 @@
         <f>AVERAGE(Table07[liczba przebytych węzłów])</f>
         <v>239335.34745762713</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="e">
+        <f>AVERAGE(Table07[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="2">
+        <f>AVERAGE(Table07[czas])</f>
+        <v>2.3910762711864413</v>
+      </c>
+      <c r="G10" s="2">
+        <f>AVERAGE(Table07[liczba króków])</f>
+        <v>3930</v>
+      </c>
+      <c r="H10" s="2" t="e">
+        <f>AVERAGE(Table07[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="2" t="e">
+        <f>AVERAGE(Table07[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <f>AVERAGE(Table07[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -6508,8 +6912,32 @@
         <f>AVERAGE(Table08[liczba przebytych węzłów])</f>
         <v>235654.0588235294</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="e">
+        <f>AVERAGE(Table08[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="2">
+        <f>AVERAGE(Table08[czas])</f>
+        <v>2.6636806722689075</v>
+      </c>
+      <c r="G11" s="2">
+        <f>AVERAGE(Table08[liczba króków])</f>
+        <v>2906.1680672268908</v>
+      </c>
+      <c r="H11" s="2" t="e">
+        <f>AVERAGE(Table08[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="2" t="e">
+        <f>AVERAGE(Table08[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <f>AVERAGE(Table08[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -6521,8 +6949,32 @@
         <f>AVERAGE(Table09[liczba przebytych węzłów])</f>
         <v>242148</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="e">
+        <f>AVERAGE(Table09[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="2">
+        <f>AVERAGE(Table09[czas])</f>
+        <v>2.6116160714285712</v>
+      </c>
+      <c r="G12" s="2">
+        <f>AVERAGE(Table09[liczba króków])</f>
+        <v>2935.8571428571427</v>
+      </c>
+      <c r="H12" s="2" t="e">
+        <f>AVERAGE(Table09[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="2" t="e">
+        <f>AVERAGE(Table09[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="2" t="e">
+        <f>AVERAGE(Table09[stan początkowy])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -6533,6 +6985,30 @@
       <c r="D13" s="2">
         <f>AVERAGE(Table10[liczba przebytych węzłów])</f>
         <v>229995.45217391304</v>
+      </c>
+      <c r="E13" s="2" t="e">
+        <f>AVERAGE(Table10[zajęta pamięć])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="2">
+        <f>AVERAGE(Table10[czas])</f>
+        <v>2.8902521739130433</v>
+      </c>
+      <c r="G13" s="2">
+        <f>AVERAGE(Table10[liczba króków])</f>
+        <v>1108.4347826086957</v>
+      </c>
+      <c r="H13" s="2" t="e">
+        <f>AVERAGE(Table10[error])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="2" t="e">
+        <f>AVERAGE(Table10[znaleziona ścieżka])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="2" t="e">
+        <f>AVERAGE(Table10[stan początkowy])</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>